<commit_message>
Minor updates, renamed spreadsheet sheet
</commit_message>
<xml_diff>
--- a/02 User Onboarding/UserUpdate.xlsx
+++ b/02 User Onboarding/UserUpdate.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\GIT\PSPlaybook-AD\02 User Onboarding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDC2D995-C2AB-4C79-8A7C-6D5447684715}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD723673-8729-467C-AB9B-EBCD770F3CF7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MOCK_DATA (6)" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1042,19 +1042,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>